<commit_message>
Corrigido um item na lista de produtos.
</commit_message>
<xml_diff>
--- a/table format.xlsx
+++ b/table format.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Semana 2" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">listaProdutos!$A$1:$H$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">listaProdutos!$A$1:$I$92</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Semana 1'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -369,9 +369,6 @@
     <t>3. Quantidade total de itens disponíveis (similar ao anterior)</t>
   </si>
   <si>
-    <t>4. Quantidade de itens disponíveis e em estoque</t>
-  </si>
-  <si>
     <t>5. Valor total do inventário da empresa (somatória dos valores individuais multiplicado pela quantidade em estoque - considere apenas os produtos “EM ESTOQUE”)</t>
   </si>
   <si>
@@ -467,6 +464,9 @@
   <si>
     <t>=INDEX(listaProdutos!B:B,MATCH(MIN(IF(listaProdutos!I2:I92&gt;0,listaProdutos!I2:I92)),listaProdutos!I:I,0))
 =INDEX(listaProdutos!H:H,MATCH(MIN(IF(listaProdutos!I2:I92&gt;0,listaProdutos!I2:I92)),listaProdutos!I:I,0))</t>
+  </si>
+  <si>
+    <t>4. Quantidade de itens disponíveis e em destaque</t>
   </si>
 </sst>
 </file>
@@ -883,7 +883,7 @@
   <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -925,7 +925,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2511,7 +2511,7 @@
         <v>3</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="I54">
         <f t="shared" si="0"/>
@@ -3659,6 +3659,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I92"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3668,7 +3669,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3735,26 +3736,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="86.21875" customWidth="1"/>
     <col min="2" max="2" width="45.88671875" customWidth="1"/>
-    <col min="3" max="3" width="88.5546875" customWidth="1"/>
+    <col min="3" max="3" width="88.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="6" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
@@ -3766,19 +3767,19 @@
         <v>2568</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="3">
         <f>SUMIF(listaProdutos!F2:F92,"sim",listaProdutos!D2:D92)</f>
         <v>2173</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
@@ -3790,91 +3791,91 @@
         <v>2568</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="B5" s="3">
-        <f>SUMIFS(listaProdutos!D2:D92,listaProdutos!D2:D92,"&gt;0",listaProdutos!E2:E92,"sim")</f>
-        <v>2568</v>
+        <f>SUMIFS(listaProdutos!D2:D92,listaProdutos!F2:F92,"sim",listaProdutos!E2:E92,"sim")</f>
+        <v>2173</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B6" s="11">
         <f>SUMPRODUCT(listaProdutos!D2:D92,listaProdutos!C2:C92)</f>
         <v>173219.55</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="12" t="str">
         <f>"Produto: "&amp;INDEX(listaProdutos!B:B,MATCH(MAX(listaProdutos!C2:C92),listaProdutos!C:C,0))&amp;" Departamento: "&amp;INDEX(listaProdutos!H:H,MATCH(MAX(listaProdutos!C2:C92),listaProdutos!C:C,0))</f>
         <v>Produto: DESKTOP ACER C24-963-UA91 I3-1005G1 1.2GHz/8GB/512GB SSD/23.8FHD IPS/W10/INGLES PRETO Departamento: Informatica</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="12" t="str">
         <f>"Produto: "&amp;INDEX(listaProdutos!B:B,MATCH(MIN(listaProdutos!C2:C92),listaProdutos!C:C,0))&amp;" Departamento: "&amp;INDEX(listaProdutos!H:H,MATCH(MIN(listaProdutos!C2:C92),listaProdutos!C:C,0))</f>
         <v>Produto: ADAPTADOR EXTENDER / RJ45 BEGE Departamento: Adaptadores</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" s="12" t="str">
         <f>"Produto: "&amp;INDEX(listaProdutos!B:B,MATCH(MAX(listaProdutos!I2:I92),listaProdutos!I:I,0))&amp;" Departamento: "&amp;INDEX(listaProdutos!H:H,MATCH(MAX(listaProdutos!I2:I92),listaProdutos!I:I,0))</f>
         <v>Produto: CONSOLE SONY PS4 SLIM 1TB CUH-2215B PRETO BIVOLT + JOGO FIFA21 EA SPORT Departamento: Games</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" s="12" t="str">
         <f t="array" ref="B10">"Produto: "&amp;INDEX(listaProdutos!B:B,MATCH(MIN(IF(listaProdutos!I2:I92&gt;0,listaProdutos!I2:I92)),listaProdutos!I:I,0))&amp;" Departamento: "&amp;INDEX(listaProdutos!H:H,MATCH(MIN(IF(listaProdutos!I2:I92&gt;0,listaProdutos!I2:I92)),listaProdutos!I:I,0))</f>
         <v>Produto: BATERIA GOLINE ALKALINE 9V 500MAH Departamento: Acessorios</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11" s="11">
         <f>B6/COUNTA(listaProdutos!B2:B92)</f>
         <v>1903.5115384615383</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -3938,19 +3939,19 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="81.33203125" customWidth="1"/>
     <col min="2" max="10" width="12" style="14" customWidth="1"/>
-    <col min="11" max="11" width="67.33203125" customWidth="1"/>
+    <col min="11" max="11" width="67.33203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>4</v>
@@ -3980,12 +3981,12 @@
         <v>97</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="3">
         <f>SUMIF(listaProdutos!$H$2:$H$92,'Semana 2'!B1,listaProdutos!$D$2:$D$92)</f>
@@ -3997,7 +3998,7 @@
       </c>
       <c r="D2" s="3">
         <f>SUMIF(listaProdutos!$H$2:$H$92,'Semana 2'!D1,listaProdutos!$D$2:$D$92)</f>
-        <v>143</v>
+        <v>227</v>
       </c>
       <c r="E2" s="3">
         <f>SUMIF(listaProdutos!$H$2:$H$92,'Semana 2'!E1,listaProdutos!$D$2:$D$92)</f>
@@ -4005,7 +4006,7 @@
       </c>
       <c r="F2" s="3">
         <f>SUMIF(listaProdutos!$H$2:$H$92,'Semana 2'!F1,listaProdutos!$D$2:$D$92)</f>
-        <v>777</v>
+        <v>693</v>
       </c>
       <c r="G2" s="3">
         <f>SUMIF(listaProdutos!$H$2:$H$92,'Semana 2'!G1,listaProdutos!$D$2:$D$92)</f>
@@ -4024,12 +4025,12 @@
         <v>195</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" s="11">
         <f>SUMIF(listaProdutos!$H$2:$H$92,'Semana 2'!B1,listaProdutos!$I$2:$I$92)</f>
@@ -4041,7 +4042,7 @@
       </c>
       <c r="D3" s="11">
         <f>SUMIF(listaProdutos!$H$2:$H$92,'Semana 2'!D1,listaProdutos!$I$2:$I$92)</f>
-        <v>9951</v>
+        <v>32043</v>
       </c>
       <c r="E3" s="11">
         <f>SUMIF(listaProdutos!$H$2:$H$92,'Semana 2'!E1,listaProdutos!$I$2:$I$92)</f>
@@ -4049,7 +4050,7 @@
       </c>
       <c r="F3" s="11">
         <f>SUMIF(listaProdutos!$H$2:$H$92,'Semana 2'!F1,listaProdutos!$I$2:$I$92)</f>
-        <v>49720.299999999996</v>
+        <v>27628.300000000003</v>
       </c>
       <c r="G3" s="11">
         <f>SUMIF(listaProdutos!$H$2:$H$92,'Semana 2'!G1,listaProdutos!$I$2:$I$92)</f>
@@ -4068,12 +4069,12 @@
         <v>5218.5999999999995</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="11">
         <f>B3/COUNTIF(listaProdutos!$H$2:$H$92,'Semana 2'!B1)</f>
@@ -4085,7 +4086,7 @@
       </c>
       <c r="D4" s="11">
         <f>D3/COUNTIF(listaProdutos!$H$2:$H$92,'Semana 2'!D1)</f>
-        <v>1243.875</v>
+        <v>3560.3333333333335</v>
       </c>
       <c r="E4" s="11">
         <f>E3/COUNTIF(listaProdutos!$H$2:$H$92,'Semana 2'!E1)</f>
@@ -4093,7 +4094,7 @@
       </c>
       <c r="F4" s="11">
         <f>F3/COUNTIF(listaProdutos!$H$2:$H$92,'Semana 2'!F1)</f>
-        <v>1775.7249999999999</v>
+        <v>1023.2703703703705</v>
       </c>
       <c r="G4" s="11">
         <f>G3/COUNTIF(listaProdutos!$H$2:$H$92,'Semana 2'!G1)</f>
@@ -4112,12 +4113,12 @@
         <v>745.51428571428562</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="3" t="str">
         <f>INDEX(B1:J1,MATCH(MAX(B3:J3),B3:J3,0))</f>
@@ -4132,12 +4133,12 @@
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
       <c r="K5" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" s="3" t="str">
         <f>INDEX(B1:J1,MATCH(MIN(B3:J3),B3:J3,0))</f>
@@ -4152,7 +4153,7 @@
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
       <c r="K6" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>